<commit_message>
Fixbug layout Change layout list messages
</commit_message>
<xml_diff>
--- a/DOCUMENT_AND_TASK_TEMP/demo_SEASOFT_laravel_nodejs_vuejs.xlsx
+++ b/DOCUMENT_AND_TASK_TEMP/demo_SEASOFT_laravel_nodejs_vuejs.xlsx
@@ -10,29 +10,17 @@
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Task detail" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
-  <si>
-    <t>Làm trang chat giống fb, list chat, khung chat</t>
-  </si>
-  <si>
-    <t>Login, logout, tạo mới user, sửa thông tin user</t>
-  </si>
-  <si>
-    <t>Chat 1-1, chat nhóm</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Ý tưởng</t>
   </si>
   <si>
     <t>Công nghệ</t>
-  </si>
-  <si>
-    <t>Vấn đề</t>
   </si>
   <si>
     <t>Thời gian</t>
@@ -104,40 +92,10 @@
     <t>https://laravel.com/docs/7.x/socialite</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Chat 1 -1 
-+ Kế thừa mọi logic từ chat room
-+ Tạo mới component cho private chat
-+ Switch được 2 component
-+ Tạo message private
-+ Load message private
-+ Tạo socket private: Chỉ emit event giữ 2 client</t>
-  </si>
-  <si>
-    <t>Xóa code thừa, xóa comment</t>
-  </si>
-  <si>
     <t>Deploy lên server, fixbug</t>
   </si>
   <si>
     <t>Checklist lại toàn bộ code, test layout, fixbug</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Run trên server thật. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="24"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Không run được là chít mịa luôn</t>
-    </r>
   </si>
   <si>
     <t>Load list user</t>
@@ -173,12 +131,73 @@
       <t>)</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">
+Chat 1 -1 
++ Kế thừa mọi logic từ chat room
++ Tạo mới component cho private chat
++ Switch được 2 component
++ Tạo message private
++ Load message private
+</t>
+  </si>
+  <si>
+    <t>Sửa giao diện</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Tạo socket private: Chỉ emit event giữ 2 client
++ Khi click vào chat, hiện tên và avatar của user bên box message
+</t>
+  </si>
+  <si>
+    <t>https://socket.io/docs/rooms/#Joining-and-leaving</t>
+  </si>
+  <si>
+    <t>(Darkmode dư thời gian thì làm)</t>
+  </si>
+  <si>
+    <t>1/ Làm trang chat giống fb, list chat, khung chat</t>
+  </si>
+  <si>
+    <t>2/ Login, logout, tạo mới user, sửa thông tin user</t>
+  </si>
+  <si>
+    <t>3/ Chat 1-1, chat nhóm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/ Làm dark mode
+2/ Test layout, responsive, test logic
+</t>
+  </si>
+  <si>
+    <t>1/ Clean code
+2/ Test</t>
+  </si>
+  <si>
+    <t>1/ Run trên server thật. 
+2/ Share link lấy data test thật</t>
+  </si>
+  <si>
+    <t>Hình minh họa</t>
+  </si>
+  <si>
+    <t>1/ Sửa lại giao diện hiện list user
+    + Hover, select tô màu user - ok
+    + Thêm button chat group - ok
+    + Show avatar user - ok
+2/ Sửa giao diện hiện list message
+      + Reply chat sẽ hiện bên trái, chính chủ hiện bên phải - ok
+     + Nhắn nhiều message chỉ hiện 1 avatar thôi  - ok
+     + Đối với chat room, hiện tên lên phía trên tin nhắn đầu tiên - ok
+      + Hiện avatar, hiện thời gian
+      + Đối với chat group hiện thêm tên người chat - ok</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,15 +221,36 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="24"/>
-      <color rgb="FFFF0000"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,18 +259,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -238,44 +284,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -291,6 +382,142 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1723129</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1038226</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="C:\Users\PHONG\AppData\Local\Temp\SNAGHTML262537ab.PNG"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8915400" y="8448675"/>
+          <a:ext cx="1675504" cy="1019176"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1114424</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1659693</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2009775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8886825" y="9544049"/>
+          <a:ext cx="1640643" cy="895351"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1685925</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3127362</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>981074</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10553700" y="8620124"/>
+          <a:ext cx="1441437" cy="790575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -580,56 +807,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.42578125" customWidth="1"/>
     <col min="2" max="2" width="66.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -640,152 +860,208 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" customWidth="1"/>
-    <col min="2" max="2" width="54.140625" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.5703125" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="54.140625" style="17" customWidth="1"/>
+    <col min="3" max="4" width="47.5703125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" style="15" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" s="24" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="20" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="20" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>44074</v>
-      </c>
-      <c r="B2" s="9" t="s">
+      <c r="C4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="1:5" s="21" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>44076</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="1:5" s="20" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>44074</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>44074</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>44075</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>44076</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>44076</v>
-      </c>
-      <c r="B8" s="9" t="s">
+      <c r="C8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+    </row>
+    <row r="9" spans="1:5" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>44077</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10"/>
+    </row>
+    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>44078</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="14"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
         <v>44079</v>
       </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="78" x14ac:dyDescent="0.5">
-      <c r="A13" s="2">
+      <c r="B12" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="18"/>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
         <v>44080</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="B13" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" display="https://www.mynotepaper.com/create-multiple-themes-in-vuejs"/>
-    <hyperlink ref="D2" r:id="rId2" display="https://www.itsolutionstuff.com/post/laravel-58-login-with-google-account-exampleexample.html"/>
-    <hyperlink ref="D8" r:id="rId3"/>
-    <hyperlink ref="D3" r:id="rId4"/>
+    <hyperlink ref="E5" r:id="rId1" display="https://www.mynotepaper.com/create-multiple-themes-in-vuejs"/>
+    <hyperlink ref="E8" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="E9" r:id="rId4" location="Joining-and-leaving"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Edit layout chat box Show name & avatar for private chat
</commit_message>
<xml_diff>
--- a/DOCUMENT_AND_TASK_TEMP/demo_SEASOFT_laravel_nodejs_vuejs.xlsx
+++ b/DOCUMENT_AND_TASK_TEMP/demo_SEASOFT_laravel_nodejs_vuejs.xlsx
@@ -99,11 +99,6 @@
   </si>
   <si>
     <t>Load list user</t>
-  </si>
-  <si>
-    <t>Load list user
- + Show name + avatar
- + Load thêm khi cuộc xuống cuối container</t>
   </si>
   <si>
     <r>
@@ -189,8 +184,13 @@
       + Reply chat sẽ hiện bên trái, chính chủ hiện bên phải - ok
      + Nhắn nhiều message chỉ hiện 1 avatar thôi  - ok
      + Đối với chat room, hiện tên lên phía trên tin nhắn đầu tiên - ok
-      + Hiện avatar, hiện thời gian
+      + Hiện avatar, hiện thời gian - ok
       + Đối với chat group hiện thêm tên người chat - ok</t>
+  </si>
+  <si>
+    <t>Load list user
+ + Show name + avatar - ok
+ + Load thêm khi cuộc xuống cuối container - ok</t>
   </si>
 </sst>
 </file>
@@ -830,7 +830,7 @@
     </row>
     <row r="2" spans="1:2" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -838,7 +838,7 @@
     </row>
     <row r="3" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -846,7 +846,7 @@
     </row>
     <row r="4" spans="1:2" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -863,8 +863,8 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,7 +887,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E1" s="23" t="s">
         <v>5</v>
@@ -931,7 +931,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="19"/>
@@ -942,7 +942,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="13" t="s">
@@ -970,7 +970,7 @@
         <v>24</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
@@ -983,7 +983,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="5" t="s">
@@ -998,11 +998,11 @@
         <v>16</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="195" x14ac:dyDescent="0.25">
@@ -1010,10 +1010,10 @@
         <v>44077</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10"/>
     </row>
@@ -1022,10 +1022,10 @@
         <v>44078</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="14"/>
     </row>
@@ -1037,7 +1037,7 @@
         <v>23</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="18"/>
     </row>
@@ -1049,7 +1049,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="18"/>
     </row>

</xml_diff>

<commit_message>
fixbug layout check email
</commit_message>
<xml_diff>
--- a/DOCUMENT_AND_TASK_TEMP/demo_SEASOFT_laravel_nodejs_vuejs.xlsx
+++ b/DOCUMENT_AND_TASK_TEMP/demo_SEASOFT_laravel_nodejs_vuejs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Ý tưởng</t>
   </si>
@@ -148,9 +148,6 @@
     <t>https://socket.io/docs/rooms/#Joining-and-leaving</t>
   </si>
   <si>
-    <t>(Darkmode dư thời gian thì làm)</t>
-  </si>
-  <si>
     <t>1/ Làm trang chat giống fb, list chat, khung chat</t>
   </si>
   <si>
@@ -158,11 +155,6 @@
   </si>
   <si>
     <t>3/ Chat 1-1, chat nhóm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/ Làm dark mode
-2/ Test layout, responsive, test logic
-</t>
   </si>
   <si>
     <t>1/ Clean code
@@ -191,6 +183,22 @@
     <t>Load list user
  + Show name + avatar - ok
  + Load thêm khi cuộc xuống cuối container - ok</t>
+  </si>
+  <si>
+    <t>Sửa giao diện, test, fixbug</t>
+  </si>
+  <si>
+    <t>(Darkmode dư thời gian thì làm) - Ko làm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/ Khi chuyển qua từng user chat, làm hiệu ứng chuyển bên khung chat - ok
+2/ Mang link socket qua file config - ok
+3/ Disconnect khi unmount vuejs component - ok (tự động hủy socket khi change component)
+4/ Check duplicate email - ok
+5/ Sửa lại logic script chổ resize, tối ưu xóa biến thừa - ok
+6/ Tách input và button send ra thì 1 component riêng
+ 7/ Room chat khi load lại, tin nhắn do mình gửi lại nằm bên trái - ok
+</t>
   </si>
 </sst>
 </file>
@@ -328,12 +336,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -369,6 +371,8 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -830,7 +834,7 @@
     </row>
     <row r="2" spans="1:2" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -838,7 +842,7 @@
     </row>
     <row r="3" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -846,7 +850,7 @@
     </row>
     <row r="4" spans="1:2" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -863,37 +867,38 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" style="17" customWidth="1"/>
-    <col min="2" max="2" width="54.140625" style="17" customWidth="1"/>
-    <col min="3" max="4" width="47.5703125" style="17" customWidth="1"/>
-    <col min="5" max="5" width="40.5703125" style="15" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="17"/>
+    <col min="1" max="1" width="31.28515625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="54.140625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="65.42578125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="47.5703125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="24" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:5" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="23" t="s">
+      <c r="D1" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44074</v>
       </c>
@@ -908,7 +913,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="20" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="18" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44074</v>
       </c>
@@ -923,7 +928,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="20" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="18" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44074</v>
       </c>
@@ -934,22 +939,22 @@
         <v>25</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="19"/>
-    </row>
-    <row r="5" spans="1:5" s="21" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12" t="s">
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" spans="1:5" s="19" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13" t="s">
+      <c r="C5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44075</v>
       </c>
@@ -960,22 +965,22 @@
         <v>15</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="19"/>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" spans="1:5" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>44076</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="1:5" s="20" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="C7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="17"/>
+    </row>
+    <row r="8" spans="1:5" s="18" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44076</v>
       </c>
@@ -990,68 +995,69 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="18" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44077</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="25"/>
+      <c r="D9" s="23"/>
       <c r="E9" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="195" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+    <row r="10" spans="1:5" s="18" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>44077</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10"/>
-    </row>
-    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="C10" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+    </row>
+    <row r="11" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>44078</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>44079</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
+        <v>44080</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="14"/>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
-        <v>44079</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
-        <v>44080</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="18"/>
+      <c r="D13" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
fixbug moment clean code
</commit_message>
<xml_diff>
--- a/DOCUMENT_AND_TASK_TEMP/demo_SEASOFT_laravel_nodejs_vuejs.xlsx
+++ b/DOCUMENT_AND_TASK_TEMP/demo_SEASOFT_laravel_nodejs_vuejs.xlsx
@@ -193,10 +193,10 @@
   <si>
     <t xml:space="preserve">1/ Khi chuyển qua từng user chat, làm hiệu ứng chuyển bên khung chat - ok
 2/ Mang link socket qua file config - ok
-3/ Disconnect khi unmount vuejs component - ok (tự động hủy socket khi change component)
+3/ Disconnect khi unmount vuejs component (tự động hủy socket khi change component) - ok
 4/ Check duplicate email - ok
 5/ Sửa lại logic script chổ resize, tối ưu xóa biến thừa - ok
-6/ Tách input và button send ra thì 1 component riêng
+6/ Tách input và button send ra thì 1 component riêng - ok
  7/ Room chat khi load lại, tin nhắn do mình gửi lại nằm bên trái - ok
 </t>
   </si>
@@ -868,7 +868,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,7 +954,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44075</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="18" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="18" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44077</v>
       </c>

</xml_diff>

<commit_message>
fixbug update user profile
</commit_message>
<xml_diff>
--- a/DOCUMENT_AND_TASK_TEMP/demo_SEASOFT_laravel_nodejs_vuejs.xlsx
+++ b/DOCUMENT_AND_TASK_TEMP/demo_SEASOFT_laravel_nodejs_vuejs.xlsx
@@ -161,10 +161,6 @@
 2/ Test</t>
   </si>
   <si>
-    <t>1/ Run trên server thật. 
-2/ Share link lấy data test thật</t>
-  </si>
-  <si>
     <t>Hình minh họa</t>
   </si>
   <si>
@@ -199,6 +195,10 @@
 6/ Tách input và button send ra thì 1 component riêng - ok
  7/ Room chat khi load lại, tin nhắn do mình gửi lại nằm bên trái - ok
 </t>
+  </si>
+  <si>
+    <t>1/ Run trên server thật. 
+2/ fixbug</t>
   </si>
 </sst>
 </file>
@@ -312,7 +312,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -364,6 +364,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -859,7 +863,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,7 +887,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>5</v>
@@ -938,7 +942,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="9" t="s">
@@ -966,7 +970,7 @@
         <v>24</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="14"/>
@@ -1009,7 +1013,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="22"/>
@@ -1019,25 +1023,26 @@
         <v>44078</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="22"/>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+    <row r="12" spans="1:5" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="23">
         <v>44079</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="13"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="22"/>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
@@ -1047,7 +1052,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D13" s="13"/>
     </row>

</xml_diff>